<commit_message>
Koodia siistitty ja kommentoitu, poistettu ääkköset taulukosta.
</commit_message>
<xml_diff>
--- a/hallitus.xlsx
+++ b/hallitus.xlsx
@@ -21,12 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
-    <t>Arvi Syrjänen</t>
-  </si>
-  <si>
-    <t>Ella Seppä</t>
-  </si>
-  <si>
     <t>Ilari Lehtinen</t>
   </si>
   <si>
@@ -39,9 +33,6 @@
     <t>Janne Siltanen</t>
   </si>
   <si>
-    <t>Jari Leppänen</t>
-  </si>
-  <si>
     <t>Jere Selkosmaa</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
     <t>Otto Saksala</t>
   </si>
   <si>
-    <t>Paula Jyrkönen</t>
-  </si>
-  <si>
     <t>Samu Ampio</t>
   </si>
   <si>
@@ -94,6 +82,18 @@
   </si>
   <si>
     <t>Viljami Tiikasalo</t>
+  </si>
+  <si>
+    <t>Arvi Syrjanen</t>
+  </si>
+  <si>
+    <t>Ella Seppa</t>
+  </si>
+  <si>
+    <t>Jari Leppanen</t>
+  </si>
+  <si>
+    <t>Paula Jyrkonen</t>
   </si>
 </sst>
 </file>
@@ -510,135 +510,135 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Korjattu virhe muuttujalistan alustuksessa
</commit_message>
<xml_diff>
--- a/hallitus.xlsx
+++ b/hallitus.xlsx
@@ -84,19 +84,19 @@
     <t>Viljami Tiikasalo</t>
   </si>
   <si>
-    <t>Arvi Syrjanen</t>
-  </si>
-  <si>
-    <t>Ella Seppa</t>
-  </si>
-  <si>
-    <t>Jari Leppanen</t>
-  </si>
-  <si>
-    <t>Paula Jyrkonen</t>
-  </si>
-  <si>
     <t>Annimari Hartikainen</t>
+  </si>
+  <si>
+    <t>Arvi Syrjänen</t>
+  </si>
+  <si>
+    <t>Ella Seppä</t>
+  </si>
+  <si>
+    <t>Jari Leppänen</t>
+  </si>
+  <si>
+    <t>Paula Jyrkönen</t>
   </si>
 </sst>
 </file>
@@ -527,20 +527,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -565,7 +568,7 @@
     </row>
     <row r="7" spans="1:1" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="40.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
@@ -628,9 +631,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -660,7 +663,7 @@
     </row>
     <row r="26" spans="1:1" ht="40.200000000000003" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>